<commit_message>
New items for patch 8.4 added
</commit_message>
<xml_diff>
--- a/private/ITEMS_1.xlsx
+++ b/private/ITEMS_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,7 +17,9 @@
     <sheet name="TRINKETS" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BOOTS!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FINAL_ITEMS!$A$1:$C$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TRINKETS!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
   <si>
     <t>Abyssal Mask</t>
   </si>
@@ -317,6 +319,15 @@
   </si>
   <si>
     <t>Enchantment: Warrior</t>
+  </si>
+  <si>
+    <t>Oblivion Orb</t>
+  </si>
+  <si>
+    <t>Spellbinder</t>
+  </si>
+  <si>
+    <t>Twin Shadows</t>
   </si>
 </sst>
 </file>
@@ -688,7 +699,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1498,6 +1509,30 @@
         <v>95</v>
       </c>
     </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>3916</v>
+      </c>
+      <c r="B96" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>3907</v>
+      </c>
+      <c r="B97" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>3905</v>
+      </c>
+      <c r="B98" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C95"/>
   <hyperlinks>
@@ -1512,10 +1547,14 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1582,6 +1621,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1590,9 +1630,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1635,6 +1681,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Oblivion Orb is not a final item
</commit_message>
<xml_diff>
--- a/private/ITEMS_1.xlsx
+++ b/private/ITEMS_1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
   <si>
     <t>Abyssal Mask</t>
   </si>
@@ -319,9 +319,6 @@
   </si>
   <si>
     <t>Enchantment: Warrior</t>
-  </si>
-  <si>
-    <t>Oblivion Orb</t>
   </si>
   <si>
     <t>Spellbinder</t>
@@ -699,7 +696,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1511,7 +1508,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>3916</v>
+        <v>3907</v>
       </c>
       <c r="B96" t="s">
         <v>96</v>
@@ -1519,18 +1516,10 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>3907</v>
+        <v>3905</v>
       </c>
       <c r="B97" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>3905</v>
-      </c>
-      <c r="B98" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shurelya's Reverie as final item added
</commit_message>
<xml_diff>
--- a/private/ITEMS_1.xlsx
+++ b/private/ITEMS_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
   <si>
     <t>Abyssal Mask</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>Twin Shadows</t>
+  </si>
+  <si>
+    <t>Shurelya's Reverie</t>
   </si>
 </sst>
 </file>
@@ -696,7 +699,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1520,6 +1523,14 @@
       </c>
       <c r="B97" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2065</v>
+      </c>
+      <c r="B98" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New perks and one new item due to patc 8.11
</commit_message>
<xml_diff>
--- a/private/ITEMS_1.xlsx
+++ b/private/ITEMS_1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAC0774-3382-40D3-8E00-3CA70359D7B8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31215" windowHeight="15675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31215" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINAL_ITEMS" sheetId="3" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
   <si>
     <t>Abyssal Mask</t>
   </si>
@@ -328,12 +329,15 @@
   </si>
   <si>
     <t>Shurelya's Reverie</t>
+  </si>
+  <si>
+    <t>Stormrazor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -698,12 +702,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,17 +1537,25 @@
         <v>98</v>
       </c>
     </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>3095</v>
+      </c>
+      <c r="B99" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C95"/>
+  <autoFilter ref="A1:C95" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1621,13 +1633,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1"/>
+  <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1681,7 +1693,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1"/>
+  <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Items and blogs updated
</commit_message>
<xml_diff>
--- a/private/ITEMS_1.xlsx
+++ b/private/ITEMS_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv\Assets\private\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv\Assets\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D1E11A-2861-4BA9-84B7-3E381547C601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73712CE-1067-465D-AFD4-3F445B00FD99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59355" yWindow="1050" windowWidth="29520" windowHeight="19020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINAL_ITEMS" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BOOTS!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FINAL_ITEMS!$A$1:$C$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FINAL_ITEMS!$A$1:$C$106</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TRINKETS!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="107">
   <si>
     <t>Abyssal Mask</t>
   </si>
@@ -347,6 +347,18 @@
   </si>
   <si>
     <t>Umbral Glaive</t>
+  </si>
+  <si>
+    <t>Black Mist Scythe</t>
+  </si>
+  <si>
+    <t>Pauldrons of Whiterock</t>
+  </si>
+  <si>
+    <t>Bulwark of the Mountain</t>
+  </si>
+  <si>
+    <t>Shard of True Ice</t>
   </si>
 </sst>
 </file>
@@ -718,11 +730,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,543 +835,549 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3153</v>
+        <v>3864</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3742</v>
+        <v>3153</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3812</v>
+        <v>3860</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3147</v>
+        <v>3742</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3814</v>
+        <v>3812</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3508</v>
+        <v>3147</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2303</v>
+        <v>3814</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2302</v>
+        <v>3508</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2301</v>
+        <v>2303</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>3401</v>
+        <v>2302</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>3092</v>
+        <v>2301</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>3110</v>
+        <v>3401</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>3022</v>
+        <v>3092</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>3193</v>
+        <v>3110</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>3026</v>
+        <v>3022</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>3124</v>
+        <v>3193</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>3030</v>
+        <v>3026</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>3146</v>
+        <v>3124</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>3152</v>
+        <v>3030</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>3025</v>
+        <v>3146</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>3031</v>
+        <v>3152</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>3109</v>
+        <v>3025</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>3151</v>
+        <v>3031</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>3100</v>
+        <v>3109</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>3190</v>
+        <v>3151</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>3036</v>
+        <v>3100</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>3104</v>
+        <v>3190</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>3285</v>
+        <v>3036</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>3004</v>
+        <v>3104</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>3156</v>
+        <v>3285</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>3041</v>
+        <v>3004</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>3139</v>
+        <v>3156</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>3222</v>
+        <v>3041</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>3170</v>
+        <v>3139</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>3165</v>
+        <v>3222</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>3033</v>
+        <v>3170</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>3115</v>
+        <v>3165</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>3056</v>
+        <v>3033</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>3198</v>
+        <v>3115</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>3046</v>
+        <v>3056</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>3089</v>
+        <v>3857</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>3143</v>
+        <v>3198</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>3094</v>
+        <v>3046</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>3074</v>
+        <v>3089</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="C54" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>3107</v>
+        <v>3143</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
-      </c>
-      <c r="C55" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>3800</v>
+        <v>3094</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>3027</v>
+        <v>3074</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>2045</v>
+        <v>3107</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="C58" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>3085</v>
+        <v>3800</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>3116</v>
+        <v>3027</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>3065</v>
+        <v>2045</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>3087</v>
+        <v>3085</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>3053</v>
+        <v>3116</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>3068</v>
+        <v>3065</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
-      </c>
-      <c r="C64" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>3069</v>
+        <v>3853</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>3071</v>
+        <v>3087</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>3072</v>
+        <v>3053</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>3185</v>
+        <v>3068</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="C68" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>3075</v>
+        <v>3069</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>3748</v>
+        <v>3071</v>
       </c>
       <c r="B70" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="C70" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>3078</v>
+        <v>3072</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>3135</v>
+        <v>3185</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>3083</v>
+        <v>3075</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>3091</v>
+        <v>3748</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>3090</v>
+        <v>3078</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C75" t="s">
         <v>86</v>
@@ -1367,225 +1385,260 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>3142</v>
+        <v>3135</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>3050</v>
+        <v>3083</v>
       </c>
       <c r="B77" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>3157</v>
+        <v>3091</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
-      </c>
-      <c r="C78" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>3512</v>
+        <v>3090</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
+        <v>3142</v>
+      </c>
+      <c r="B80" t="s">
+        <v>79</v>
+      </c>
+      <c r="C80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>3050</v>
+      </c>
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>3157</v>
+      </c>
+      <c r="B82" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>3512</v>
+      </c>
+      <c r="B83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
         <v>1419</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B84" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
         <v>1418</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B85" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
         <v>3675</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B86" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
         <v>1416</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B87" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
         <v>1409</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B88" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
         <v>1401</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B89" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
         <v>3672</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B90" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
         <v>1413</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B91" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
         <v>1414</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B92" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
         <v>1410</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B93" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
         <v>3673</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B94" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
         <v>1402</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B95" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
         <v>1400</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B96" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>3671</v>
-      </c>
-      <c r="B93" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>1412</v>
-      </c>
-      <c r="B94" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>1408</v>
-      </c>
-      <c r="B95" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>3907</v>
-      </c>
-      <c r="B96" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>3905</v>
+        <v>3671</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>2065</v>
+        <v>1412</v>
       </c>
       <c r="B98" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>3095</v>
+        <v>1408</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>3161</v>
+        <v>3907</v>
       </c>
       <c r="B100" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>3181</v>
+        <v>3905</v>
       </c>
       <c r="B101" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
+        <v>2065</v>
+      </c>
+      <c r="B102" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>3095</v>
+      </c>
+      <c r="B103" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>3161</v>
+      </c>
+      <c r="B104" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>3181</v>
+      </c>
+      <c r="B105" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
         <v>3179</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B106" t="s">
         <v>102</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C102" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C106" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
new preseason finished items added
</commit_message>
<xml_diff>
--- a/private/ITEMS_1.xlsx
+++ b/private/ITEMS_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv\Assets\Assets\private\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv1\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73712CE-1067-465D-AFD4-3F445B00FD99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6C0D6D-73B6-4B30-B372-4E8CF6FD189B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINAL_ITEMS" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="140">
   <si>
     <t>Abyssal Mask</t>
   </si>
@@ -359,6 +359,105 @@
   </si>
   <si>
     <t>Shard of True Ice</t>
+  </si>
+  <si>
+    <t>Staff of Flowing Water</t>
+  </si>
+  <si>
+    <t>Force of Nature</t>
+  </si>
+  <si>
+    <t>Chempunk Chainsword</t>
+  </si>
+  <si>
+    <t>Chemtech Putrifier</t>
+  </si>
+  <si>
+    <t>Cosmic Drive</t>
+  </si>
+  <si>
+    <t>Demonic Embrace</t>
+  </si>
+  <si>
+    <t>Divine Sunderer</t>
+  </si>
+  <si>
+    <t>Eclipse</t>
+  </si>
+  <si>
+    <t>Everfrost</t>
+  </si>
+  <si>
+    <t>Frostfire Gauntlet</t>
+  </si>
+  <si>
+    <t>Galeforce</t>
+  </si>
+  <si>
+    <t>Goredrinker</t>
+  </si>
+  <si>
+    <t>Hextech Rocketbelt</t>
+  </si>
+  <si>
+    <t>Horizon Focus</t>
+  </si>
+  <si>
+    <t>Immortal Shieldbow</t>
+  </si>
+  <si>
+    <t>Imperial Mandate</t>
+  </si>
+  <si>
+    <t>Kraken Slayer</t>
+  </si>
+  <si>
+    <t>Liandry's Anguish</t>
+  </si>
+  <si>
+    <t>Luden's Tempest</t>
+  </si>
+  <si>
+    <t>Mikael's Blessing</t>
+  </si>
+  <si>
+    <t>Moonstone Renewer</t>
+  </si>
+  <si>
+    <t>Navori Quickblades</t>
+  </si>
+  <si>
+    <t>Night Harvester</t>
+  </si>
+  <si>
+    <t>Prowler's Claw</t>
+  </si>
+  <si>
+    <t>Riftmaker</t>
+  </si>
+  <si>
+    <t>Serpent's Fang</t>
+  </si>
+  <si>
+    <t>Serylda's Grudge</t>
+  </si>
+  <si>
+    <t>Shurelya's Battlesong</t>
+  </si>
+  <si>
+    <t>Silvermere Dawn</t>
+  </si>
+  <si>
+    <t>Stridebreaker</t>
+  </si>
+  <si>
+    <t>Sunfire Aegis</t>
+  </si>
+  <si>
+    <t>The Collector</t>
+  </si>
+  <si>
+    <t>Turbo Chemtank</t>
   </si>
 </sst>
 </file>
@@ -730,11 +829,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,7 +1656,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>3671</v>
       </c>
@@ -1565,7 +1664,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1412</v>
       </c>
@@ -1573,7 +1672,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1408</v>
       </c>
@@ -1581,7 +1680,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>3907</v>
       </c>
@@ -1589,7 +1688,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>3905</v>
       </c>
@@ -1597,7 +1696,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2065</v>
       </c>
@@ -1605,7 +1704,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>3095</v>
       </c>
@@ -1613,7 +1712,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>3161</v>
       </c>
@@ -1621,7 +1720,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>3181</v>
       </c>
@@ -1629,12 +1728,355 @@
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>3179</v>
       </c>
       <c r="B106" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>6333</v>
+      </c>
+      <c r="B107" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>6691</v>
+      </c>
+      <c r="B108" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>6616</v>
+      </c>
+      <c r="B109" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>4401</v>
+      </c>
+      <c r="B110" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>6609</v>
+      </c>
+      <c r="B111" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>3011</v>
+      </c>
+      <c r="B112" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>4629</v>
+      </c>
+      <c r="B113" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>4637</v>
+      </c>
+      <c r="B114" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>6632</v>
+      </c>
+      <c r="B115" t="s">
+        <v>113</v>
+      </c>
+      <c r="C115" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>6692</v>
+      </c>
+      <c r="B116" t="s">
+        <v>114</v>
+      </c>
+      <c r="C116" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>6656</v>
+      </c>
+      <c r="B117" t="s">
+        <v>115</v>
+      </c>
+      <c r="C117" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>6662</v>
+      </c>
+      <c r="B118" t="s">
+        <v>116</v>
+      </c>
+      <c r="C118" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>6671</v>
+      </c>
+      <c r="B119" t="s">
+        <v>117</v>
+      </c>
+      <c r="C119" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>6630</v>
+      </c>
+      <c r="B120" t="s">
+        <v>118</v>
+      </c>
+      <c r="C120" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>3152</v>
+      </c>
+      <c r="B121" t="s">
+        <v>119</v>
+      </c>
+      <c r="C121" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>4628</v>
+      </c>
+      <c r="B122" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>6673</v>
+      </c>
+      <c r="B123" t="s">
+        <v>121</v>
+      </c>
+      <c r="C123" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>4005</v>
+      </c>
+      <c r="B124" t="s">
+        <v>122</v>
+      </c>
+      <c r="C124" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>6672</v>
+      </c>
+      <c r="B125" t="s">
+        <v>123</v>
+      </c>
+      <c r="C125" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>6653</v>
+      </c>
+      <c r="B126" t="s">
+        <v>124</v>
+      </c>
+      <c r="C126" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>6655</v>
+      </c>
+      <c r="B127" t="s">
+        <v>125</v>
+      </c>
+      <c r="C127" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>3222</v>
+      </c>
+      <c r="B128" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>6617</v>
+      </c>
+      <c r="B129" t="s">
+        <v>127</v>
+      </c>
+      <c r="C129" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>6675</v>
+      </c>
+      <c r="B130" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>4636</v>
+      </c>
+      <c r="B131" t="s">
+        <v>129</v>
+      </c>
+      <c r="C131" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>6693</v>
+      </c>
+      <c r="B132" t="s">
+        <v>130</v>
+      </c>
+      <c r="C132" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>4633</v>
+      </c>
+      <c r="B133" t="s">
+        <v>131</v>
+      </c>
+      <c r="C133" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>6695</v>
+      </c>
+      <c r="B134" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>6694</v>
+      </c>
+      <c r="B135" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>2065</v>
+      </c>
+      <c r="B136" t="s">
+        <v>134</v>
+      </c>
+      <c r="C136" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>6035</v>
+      </c>
+      <c r="B137" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>6631</v>
+      </c>
+      <c r="B138" t="s">
+        <v>136</v>
+      </c>
+      <c r="C138" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>3068</v>
+      </c>
+      <c r="B139" t="s">
+        <v>137</v>
+      </c>
+      <c r="C139" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>6676</v>
+      </c>
+      <c r="B140" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>6664</v>
+      </c>
+      <c r="B141" t="s">
+        <v>139</v>
+      </c>
+      <c r="C141" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>